<commit_message>
Added files for lab3
</commit_message>
<xml_diff>
--- a/Lab 2/Book1.xlsx
+++ b/Lab 2/Book1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2cd3e99d6a3c3959/Documents/2017 UBC/ELEC 291/Lab 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mansu\OneDrive\Documents\2017 UBC\ELEC 291\Lab 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="975" yWindow="0" windowWidth="27825" windowHeight="12795"/>
+    <workbookView xWindow="980" yWindow="460" windowWidth="27830" windowHeight="12800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Note</t>
   </si>
@@ -412,15 +412,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E19"/>
+  <dimension ref="B2:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -434,7 +434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -450,7 +450,7 @@
         <v>60252.101290014332</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -458,15 +458,15 @@
         <v>2349.3200000000002</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D19" si="0">C4*2</f>
+        <f t="shared" ref="D4:D9" si="0">C4*2</f>
         <v>4698.6400000000003</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E19" si="1">65536-(22118400/D4)</f>
+        <f t="shared" ref="E4:E9" si="1">65536-(22118400/D4)</f>
         <v>60828.595304173126</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -482,7 +482,7 @@
         <v>61342.175152255193</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -498,7 +498,7 @@
         <v>61577.563015645188</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -514,7 +514,7 @@
         <v>62009.424405923543</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -530,7 +530,7 @@
         <v>62394.181818181816</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -546,147 +546,163 @@
         <v>62736.960752403778</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>4186</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10" si="2">C10*2</f>
+        <v>8372</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" ref="E10" si="3">65536-(22118400/D10)</f>
+        <v>62894.05064500717</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>2637.02</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
+      <c r="D12">
+        <f>C12*2</f>
         <v>5274.04</v>
       </c>
-      <c r="E11" s="1">
-        <f t="shared" si="1"/>
+      <c r="E12" s="1">
+        <f>65536-(22118400/D12)</f>
         <v>61342.175152255193</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>2489.02</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
+      <c r="D13">
+        <f>C13*2</f>
         <v>4978.04</v>
       </c>
-      <c r="E12" s="1">
-        <f t="shared" si="1"/>
+      <c r="E13" s="1">
+        <f>65536-(22118400/D13)</f>
         <v>61092.805489710809</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>2637.02</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
+      <c r="D14">
+        <f>C14*2</f>
         <v>5274.04</v>
       </c>
-      <c r="E13" s="1">
-        <f t="shared" si="1"/>
+      <c r="E14" s="1">
+        <f>65536-(22118400/D14)</f>
         <v>61342.175152255193</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>2489.02</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
+      <c r="D15">
+        <f>C15*2</f>
         <v>4978.04</v>
       </c>
-      <c r="E14" s="1">
-        <f t="shared" si="1"/>
+      <c r="E15" s="1">
+        <f>65536-(22118400/D15)</f>
         <v>61092.805489710809</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>2637.02</v>
       </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
+      <c r="D16">
+        <f>C16*2</f>
         <v>5274.04</v>
-      </c>
-      <c r="E15" s="1">
-        <f t="shared" si="1"/>
-        <v>61342.175152255193</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16">
-        <v>1975.53</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>3951.06</v>
       </c>
       <c r="E16" s="1">
         <f>65536-(22118400/D16)</f>
+        <v>61342.175152255193</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>1975.53</v>
+      </c>
+      <c r="D17">
+        <f>C17*2</f>
+        <v>3951.06</v>
+      </c>
+      <c r="E17" s="1">
+        <f>65536-(22118400/D17)</f>
         <v>59937.90733625913</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>2349.3200000000002</v>
       </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
+      <c r="D18">
+        <f>C18*2</f>
         <v>4698.6400000000003</v>
       </c>
-      <c r="E17" s="1">
-        <f t="shared" si="1"/>
+      <c r="E18" s="1">
+        <f>65536-(22118400/D18)</f>
         <v>60828.595304173126</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
         <v>5</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>2093</v>
       </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
+      <c r="D19">
+        <f>C19*2</f>
         <v>4186</v>
       </c>
-      <c r="E18" s="1">
-        <f t="shared" si="1"/>
+      <c r="E19" s="1">
+        <f>65536-(22118400/D19)</f>
         <v>60252.101290014332</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
         <v>3</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>1760</v>
       </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
+      <c r="D20">
+        <f>C20*2</f>
         <v>3520</v>
       </c>
-      <c r="E19" s="1">
-        <f t="shared" si="1"/>
+      <c r="E20" s="1">
+        <f>65536-(22118400/D20)</f>
         <v>59252.363636363632</v>
       </c>
     </row>

</xml_diff>